<commit_message>
add rpt day sum
</commit_message>
<xml_diff>
--- a/guilde.xlsx
+++ b/guilde.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tmp\github\accounting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="foler structure" sheetId="1" r:id="rId1"/>
@@ -18,8 +13,9 @@
     <sheet name="s.2" sheetId="3" r:id="rId4"/>
     <sheet name="config" sheetId="4" r:id="rId5"/>
     <sheet name="edit" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
   <si>
     <t>Cấu trúc thư mục</t>
   </si>
@@ -302,6 +298,42 @@
   </si>
   <si>
     <t>hoặc nhấn nút "X" để hủy bỏ</t>
+  </si>
+  <si>
+    <t>mã phiếu thu</t>
+  </si>
+  <si>
+    <t>mẫ phiếu chi</t>
+  </si>
+  <si>
+    <t>rcpt_20180102_001</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>rcpt_yyyyMMdd_nnn</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>phiếu thu số 1 ngày 2/1/2018</t>
+  </si>
+  <si>
+    <t>lương</t>
+  </si>
+  <si>
+    <t>sala_xxx</t>
+  </si>
+  <si>
+    <t>inpm_xxx</t>
+  </si>
+  <si>
+    <t>expm_xxx</t>
   </si>
 </sst>
 </file>
@@ -9040,7 +9072,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9075,7 +9107,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9252,7 +9284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9818,7 +9850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I115"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
+    <sheetView topLeftCell="A101" workbookViewId="0">
       <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
@@ -11708,7 +11740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
@@ -11803,7 +11835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -11866,4 +11898,65 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>